<commit_message>
AA - Update for inputs
</commit_message>
<xml_diff>
--- a/data/support_trascodifiche.xlsx
+++ b/data/support_trascodifiche.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://innovationteam-my.sharepoint.com/personal/a_abraham_innovationteam_eu/Documents/Documenti/progetti/22p11_Tool_FA/inputs_mod/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://innovationteam-my.sharepoint.com/personal/a_abraham_innovationteam_eu/Documents/Documenti/progetti/22p11_Tool_FA_production/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:1_{54BC2D7E-0A9F-44CA-9791-8F1FA2B4139E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7A6516E-245B-4802-88C3-9D998F28AB32}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{54BC2D7E-0A9F-44CA-9791-8F1FA2B4139E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80EAB8A0-4BDA-43A7-850B-80F25D3AE024}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" firstSheet="1" activeTab="4" xr2:uid="{9758A490-5BBA-4DAE-A128-35FF12EB83CB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" firstSheet="1" activeTab="3" xr2:uid="{9758A490-5BBA-4DAE-A128-35FF12EB83CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Condizioni_Commerciali" sheetId="7" r:id="rId1"/>
@@ -7592,8 +7592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1108AB1-127A-4D50-9F30-C7486AA9E608}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7735,8 +7735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F3E4911-66FD-46BA-85EE-7208A8CAC824}">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F113" sqref="F113"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>